<commit_message>
added cindex values from system branches to main summary sheet for better transparency
</commit_message>
<xml_diff>
--- a/codecarbon_results_evaluation.xlsx
+++ b/codecarbon_results_evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Offiziell\Informatik\Master\2024SS\HCAI\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cloudsync\Shares\research\2025_appliedsciences-revision\Figures_NEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E230EC-2217-44BF-91B3-54A03C9E1390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950CE107-80F6-4DE3-8C65-AC09474A2B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="602" firstSheet="4" activeTab="8" xr2:uid="{EE9CF6A2-73EE-40C4-A7D2-03E2ABF87997}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="683" firstSheet="4" activeTab="5" xr2:uid="{EE9CF6A2-73EE-40C4-A7D2-03E2ABF87997}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Emissions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,32 @@
     <sheet name="System Comparison" sheetId="4" r:id="rId7"/>
     <sheet name="CC Output expl" sheetId="5" r:id="rId8"/>
     <sheet name="Dashboard Comparisons" sheetId="9" r:id="rId9"/>
+    <sheet name="c-indices" sheetId="10" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'c-indices'!$I$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'c-indices'!$I$4:$I$18</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'c-indices'!$N$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'c-indices'!$N$4:$N$18</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'c-indices'!$O$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'c-indices'!$O$4:$O$18</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'c-indices'!$P$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'c-indices'!$P$4:$P$18</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'c-indices'!$Q$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'c-indices'!$Q$4:$Q$18</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'c-indices'!$R$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'c-indices'!$R$4:$R$18</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'c-indices'!$J$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'c-indices'!$S$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'c-indices'!$S$4:$S$18</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'c-indices'!$J$4:$J$18</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'c-indices'!$K$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'c-indices'!$K$4:$K$18</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'c-indices'!$L$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'c-indices'!$L$4:$L$18</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'c-indices'!$M$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'c-indices'!$M$4:$M$18</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -337,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="272">
   <si>
     <t>timestamp</t>
   </si>
@@ -1250,6 +1275,60 @@
   </si>
   <si>
     <t>Calculation of Metrics from Examples</t>
+  </si>
+  <si>
+    <t>system1</t>
+  </si>
+  <si>
+    <t>system2</t>
+  </si>
+  <si>
+    <t>2layer</t>
+  </si>
+  <si>
+    <t>3layer</t>
+  </si>
+  <si>
+    <t>4layer</t>
+  </si>
+  <si>
+    <t>pathway</t>
+  </si>
+  <si>
+    <t>no_pathway</t>
+  </si>
+  <si>
+    <t>coxph</t>
+  </si>
+  <si>
+    <t>stbw</t>
+  </si>
+  <si>
+    <t>mw</t>
+  </si>
+  <si>
+    <t>piDeeL</t>
+  </si>
+  <si>
+    <t>rsf</t>
+  </si>
+  <si>
+    <t>system 2</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>extracted data from Figure 2 in original study by Kaynar et al 2023</t>
   </si>
 </sst>
 </file>
@@ -1748,7 +1827,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1985,6 +2064,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2038,7 +2124,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2070,7 +2156,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2454,7 +2540,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2518,13 +2604,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-AT"/>
-                  <a:t>duration</a:t>
+                  <a:t>duration [s]</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-AT" baseline="0"/>
-                  <a:t> [s]</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-AT"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2553,7 +2634,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="de-AT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2573,7 +2654,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2608,8 +2689,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.67976629791278675"/>
           <c:y val="2.1064153485239157E-2"/>
-          <c:w val="0.22958361343599137"/>
-          <c:h val="6.5762354926873073E-2"/>
+          <c:w val="0.30087764453172167"/>
+          <c:h val="7.5205215141308471E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2625,7 +2706,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2650,12 +2731,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2665,7 +2741,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1000"/>
       </a:pPr>
       <a:endParaRPr lang="de-DE"/>
     </a:p>
@@ -3215,7 +3291,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="de-AT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3270,8 +3346,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.6810559548640378"/>
           <c:y val="2.1064153485239157E-2"/>
-          <c:w val="0.22829395648474038"/>
-          <c:h val="6.5762354926873073E-2"/>
+          <c:w val="0.23771011674388154"/>
+          <c:h val="8.9369521090316983E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3312,12 +3388,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -3926,8 +3997,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.68621458266904167"/>
           <c:y val="2.1064153485239157E-2"/>
-          <c:w val="0.22313532867973654"/>
-          <c:h val="6.5762354926873073E-2"/>
+          <c:w val="0.2379322288103817"/>
+          <c:h val="7.992665045764466E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3968,12 +4039,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -4585,8 +4651,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.68234561181528874"/>
           <c:y val="2.1064153485239157E-2"/>
-          <c:w val="0.22700429953348941"/>
-          <c:h val="6.5762354926873073E-2"/>
+          <c:w val="0.23373010577067702"/>
+          <c:h val="8.2287368115812734E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -4627,12 +4693,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -5958,8 +6019,8 @@
           <c:yMode val="edge"/>
           <c:x val="1.5564229993561872E-2"/>
           <c:y val="5.7937309827422005E-2"/>
-          <c:w val="0.22482234213888083"/>
-          <c:h val="6.0841288644229191E-2"/>
+          <c:w val="0.23558368763226631"/>
+          <c:h val="7.0284141182068952E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -6000,12 +6061,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -7417,8 +7473,8 @@
           <c:yMode val="edge"/>
           <c:x val="1.5906852241870596E-2"/>
           <c:y val="7.0151495593602217E-2"/>
-          <c:w val="0.22236681499414068"/>
-          <c:h val="8.2965182449538946E-2"/>
+          <c:w val="0.23312816830099628"/>
+          <c:h val="6.4079357289970496E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -7459,12 +7515,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -8069,8 +8120,8 @@
           <c:yMode val="edge"/>
           <c:x val="5.8902785320162368E-2"/>
           <c:y val="7.0151547837342246E-2"/>
-          <c:w val="0.31125748834826611"/>
-          <c:h val="9.0753963973681379E-2"/>
+          <c:w val="0.32644312700091555"/>
+          <c:h val="6.8432578740157485E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -8806,12 +8857,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -8832,6 +8878,442 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="4">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="5">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.11</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="6">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="7">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="8">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.17</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="9">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.19</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="10">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.21</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{3C6895CF-A6B8-4868-AEE5-4A7D70343568}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:v>piDeeL</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{5B252D88-9DA6-42B0-A972-113DAA949BC8}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>coxph</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{9F74F6EF-D34A-4A91-AE81-8B9B6EC68689}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>rsf</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{DC829C6B-E3CE-43D0-8CCB-1A7C6BD73AA7}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:v/>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{4F5E367A-74C8-4B1B-A087-FE1DF5CC8C9D}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:v>piDeeL</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="4"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{E286DDDA-6781-430A-9147-44BB553FC272}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:v>coxph</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="5"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{755BECD9-D93A-4E27-9682-CF5A5A15271F}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:v>rsf</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B0F0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="6"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{1229224F-89A2-4B41-A593-7C497ADED602}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v/>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="7"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{AEEA8E23-02F8-45CE-86DB-473F0C996718}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:v>piDeeL</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="8"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{2DEC3BE3-DB93-44D1-81FF-02B0D1CD0B89}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:v>coxph</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="9"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{27B7F894-E609-4BC3-844F-1ABE5D741E3E}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:v>rsf</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </cx:spPr>
+          <cx:dataId val="10"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="0"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>system</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1600">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Open Sans Bold"/>
+                  <a:ea typeface="Open Sans Bold"/>
+                  <a:cs typeface="Open Sans Bold"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Open Sans Bold"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>system</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1600" b="0" i="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Open Sans Bold"/>
+                <a:ea typeface="Open Sans Bold"/>
+                <a:cs typeface="Open Sans Bold"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-AT" sz="1600">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Open Sans Bold"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling min="0.5"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>c-index</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1600">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Open Sans Bold"/>
+                  <a:ea typeface="Open Sans Bold"/>
+                  <a:cs typeface="Open Sans Bold"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Open Sans Bold"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>c-index</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1200" b="0" i="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Open Sans Bold"/>
+                <a:ea typeface="Open Sans Bold"/>
+                <a:cs typeface="Open Sans Bold"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-AT" sz="1200">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Open Sans Bold"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+  <cx:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </cx:spPr>
+</cx:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9154,6 +9636,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -13174,6 +13696,521 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -13487,6 +14524,89 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>530225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>530225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Diagramm 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F071177-DDB7-2269-AC98-06F3752F05DB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5699125" y="457200"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-AT" sz="1100"/>
+                <a:t>Dieses Diagramm ist in Ihrer Version von Excel nicht verfügbar.
+Wenn Sie diese Form bearbeiten oder diese Arbeitsmappe in einem anderen Dateiformat speichern, wird das Diagramm dauerhaft beschädigt.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -13790,42 +14910,42 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.21875" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="26" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="35.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.88671875" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" style="26" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="26" customWidth="1"/>
-    <col min="14" max="15" width="10.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.26953125" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" style="26" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="35.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.81640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" style="26" customWidth="1"/>
+    <col min="11" max="11" width="19.7265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7265625" style="26" customWidth="1"/>
+    <col min="14" max="15" width="10.1796875" style="26" bestFit="1" customWidth="1"/>
     <col min="16" max="19" width="12" style="26" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.77734375" style="26" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.77734375" style="26" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5546875" style="26" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="6.109375" style="26" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="13.21875" style="26" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5546875" style="26" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="55.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.5546875" style="26" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="17.6640625" style="26" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="9.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="41.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="38.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5546875" style="26" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="7.21875" style="26" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="13.109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.109375" style="26" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="8.5546875" style="26" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7265625" style="26" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="15.54296875" style="26" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="6.1796875" style="26" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="13.26953125" style="26" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="11.54296875" style="26" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="55.7265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.54296875" style="26" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="17.7265625" style="26" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="9.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="41.26953125" style="26" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="38.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.54296875" style="26" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="7.26953125" style="26" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="13.1796875" style="26" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.1796875" style="26" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="8.54296875" style="26" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="4" style="26" hidden="1" customWidth="1"/>
-    <col min="39" max="16384" width="11.5546875" style="26"/>
+    <col min="39" max="16384" width="11.54296875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -14277,6 +15397,1494 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6CCC64-30A8-48D8-9B7D-7C3EF808CB06}">
+  <dimension ref="B1:U41"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="2.81640625" style="68" customWidth="1"/>
+    <col min="2" max="2" width="5.7265625" style="68" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" style="68" customWidth="1"/>
+    <col min="4" max="16384" width="10.90625" style="68"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21">
+      <c r="C1" s="68" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>258</v>
+      </c>
+      <c r="I1" s="68" t="s">
+        <v>264</v>
+      </c>
+      <c r="J1" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="K1" s="68" t="s">
+        <v>265</v>
+      </c>
+      <c r="M1" s="68" t="s">
+        <v>264</v>
+      </c>
+      <c r="N1" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="O1" s="68" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q1" s="68" t="s">
+        <v>264</v>
+      </c>
+      <c r="R1" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="S1" s="68" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21">
+      <c r="C2" s="68" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" s="68" t="s">
+        <v>260</v>
+      </c>
+      <c r="I2" s="68" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q2" s="68" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21">
+      <c r="I3" s="68" t="s">
+        <v>254</v>
+      </c>
+      <c r="M3" s="68" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q3" s="68" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21">
+      <c r="B4" s="89" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="90">
+        <v>0.59380200000000005</v>
+      </c>
+      <c r="D4" s="90">
+        <v>0.56900799999999996</v>
+      </c>
+      <c r="E4" s="90">
+        <v>0.573967</v>
+      </c>
+      <c r="F4" s="90">
+        <v>0.59421500000000005</v>
+      </c>
+      <c r="G4" s="90">
+        <v>0.57768600000000003</v>
+      </c>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90">
+        <v>0.61198300000000005</v>
+      </c>
+      <c r="J4">
+        <v>0.61618300000000004</v>
+      </c>
+      <c r="K4">
+        <v>0.54481299999999999</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4" s="90">
+        <v>0.58388399999999996</v>
+      </c>
+      <c r="N4">
+        <v>0.61618300000000004</v>
+      </c>
+      <c r="O4">
+        <v>0.54481299999999999</v>
+      </c>
+      <c r="P4" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q4" s="68">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="R4">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="S4" s="68">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="T4" s="88"/>
+    </row>
+    <row r="5" spans="2:21">
+      <c r="C5" s="90">
+        <v>0.49695800000000001</v>
+      </c>
+      <c r="D5" s="90">
+        <v>0.59809900000000005</v>
+      </c>
+      <c r="E5" s="90">
+        <v>0.56996199999999997</v>
+      </c>
+      <c r="F5" s="90">
+        <v>0.55703400000000003</v>
+      </c>
+      <c r="G5" s="90">
+        <v>0.50760499999999997</v>
+      </c>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90">
+        <v>0.59581700000000004</v>
+      </c>
+      <c r="J5">
+        <v>0.62062399999999995</v>
+      </c>
+      <c r="K5">
+        <v>0.61567700000000003</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5" s="90">
+        <v>0.62281399999999998</v>
+      </c>
+      <c r="N5">
+        <v>0.62062399999999995</v>
+      </c>
+      <c r="O5">
+        <v>0.61567700000000003</v>
+      </c>
+      <c r="P5" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q5" s="68">
+        <v>0.628</v>
+      </c>
+      <c r="R5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="S5">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="T5" s="88"/>
+      <c r="U5" s="88"/>
+    </row>
+    <row r="6" spans="2:21">
+      <c r="C6" s="90">
+        <v>0.59196499999999996</v>
+      </c>
+      <c r="D6" s="90">
+        <v>0.56085099999999999</v>
+      </c>
+      <c r="E6" s="90">
+        <v>0.59511599999999998</v>
+      </c>
+      <c r="F6" s="90">
+        <v>0.58842099999999997</v>
+      </c>
+      <c r="G6" s="90">
+        <v>0.57699900000000004</v>
+      </c>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90">
+        <v>0.59629799999999999</v>
+      </c>
+      <c r="J6">
+        <v>0.60850700000000002</v>
+      </c>
+      <c r="K6">
+        <v>0.56203199999999998</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6" s="90">
+        <v>0.59472199999999997</v>
+      </c>
+      <c r="N6">
+        <v>0.60850700000000002</v>
+      </c>
+      <c r="O6">
+        <v>0.56242599999999998</v>
+      </c>
+      <c r="P6" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q6">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R6">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="S6">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="T6" s="88"/>
+      <c r="U6" s="88"/>
+    </row>
+    <row r="7" spans="2:21">
+      <c r="C7" s="90">
+        <v>0.72649600000000003</v>
+      </c>
+      <c r="D7" s="90">
+        <v>0.72820499999999999</v>
+      </c>
+      <c r="E7" s="90">
+        <v>0.72606800000000005</v>
+      </c>
+      <c r="F7" s="90">
+        <v>0.72649600000000003</v>
+      </c>
+      <c r="G7" s="90">
+        <v>0.72307699999999997</v>
+      </c>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90">
+        <v>0.70940199999999998</v>
+      </c>
+      <c r="J7">
+        <v>0.72509599999999996</v>
+      </c>
+      <c r="K7">
+        <v>0.598333</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7" s="90">
+        <v>0.69359000000000004</v>
+      </c>
+      <c r="N7">
+        <v>0.72509599999999996</v>
+      </c>
+      <c r="O7">
+        <v>0.598333</v>
+      </c>
+      <c r="P7"/>
+      <c r="R7">
+        <v>0.59</v>
+      </c>
+      <c r="S7">
+        <v>0.69833299999999998</v>
+      </c>
+      <c r="T7" s="88"/>
+      <c r="U7" s="88"/>
+    </row>
+    <row r="8" spans="2:21">
+      <c r="C8" s="90">
+        <v>0.64832100000000004</v>
+      </c>
+      <c r="D8" s="90">
+        <v>0.63536999999999999</v>
+      </c>
+      <c r="E8" s="90">
+        <v>0.61837299999999995</v>
+      </c>
+      <c r="F8" s="90">
+        <v>0.63010900000000003</v>
+      </c>
+      <c r="G8" s="90">
+        <v>0.63860799999999995</v>
+      </c>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90">
+        <v>0.60623199999999999</v>
+      </c>
+      <c r="J8">
+        <v>0.65532599999999996</v>
+      </c>
+      <c r="K8">
+        <v>0.64803599999999995</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8" s="90">
+        <v>0.62080100000000005</v>
+      </c>
+      <c r="N8">
+        <v>0.65532599999999996</v>
+      </c>
+      <c r="O8">
+        <v>0.64803599999999995</v>
+      </c>
+      <c r="P8"/>
+      <c r="Q8">
+        <v>0.69</v>
+      </c>
+      <c r="R8">
+        <v>0.64803599999999995</v>
+      </c>
+      <c r="S8">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="T8" s="88"/>
+      <c r="U8" s="88"/>
+    </row>
+    <row r="9" spans="2:21">
+      <c r="C9" s="90">
+        <v>0.45760899999999999</v>
+      </c>
+      <c r="D9" s="90">
+        <v>0.59420300000000004</v>
+      </c>
+      <c r="E9" s="90">
+        <v>0.59492800000000001</v>
+      </c>
+      <c r="F9" s="90">
+        <v>0.59673900000000002</v>
+      </c>
+      <c r="G9" s="90">
+        <v>0.56702900000000001</v>
+      </c>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90">
+        <v>0.57101400000000002</v>
+      </c>
+      <c r="J9">
+        <v>0.64078400000000002</v>
+      </c>
+      <c r="K9">
+        <v>0.59433999999999998</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9" s="90">
+        <v>0.57536200000000004</v>
+      </c>
+      <c r="N9">
+        <v>0.64078400000000002</v>
+      </c>
+      <c r="O9">
+        <v>0.59433999999999998</v>
+      </c>
+      <c r="P9"/>
+      <c r="Q9" s="68">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="R9">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="S9">
+        <v>0.627</v>
+      </c>
+      <c r="T9" s="88"/>
+      <c r="U9" s="88"/>
+    </row>
+    <row r="10" spans="2:21">
+      <c r="C10" s="90">
+        <v>0.632911</v>
+      </c>
+      <c r="D10" s="90">
+        <v>0.61457899999999999</v>
+      </c>
+      <c r="E10" s="90">
+        <v>0.60803099999999999</v>
+      </c>
+      <c r="F10" s="90">
+        <v>0.616761</v>
+      </c>
+      <c r="G10" s="90">
+        <v>0.61894400000000005</v>
+      </c>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90">
+        <v>0.608904</v>
+      </c>
+      <c r="J10">
+        <v>0.71534799999999998</v>
+      </c>
+      <c r="K10">
+        <v>0.57586400000000004</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10" s="90">
+        <v>0.62461800000000001</v>
+      </c>
+      <c r="N10">
+        <v>0.71534799999999998</v>
+      </c>
+      <c r="O10">
+        <v>0.57586400000000004</v>
+      </c>
+      <c r="P10"/>
+      <c r="R10" s="68">
+        <v>0.65</v>
+      </c>
+      <c r="S10">
+        <v>0.66</v>
+      </c>
+      <c r="T10" s="88"/>
+      <c r="U10" s="88"/>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="C11" s="90">
+        <v>0.59164499999999998</v>
+      </c>
+      <c r="D11" s="90">
+        <v>0.60144900000000001</v>
+      </c>
+      <c r="E11" s="90">
+        <v>0.59462899999999996</v>
+      </c>
+      <c r="F11" s="90">
+        <v>0.58610399999999996</v>
+      </c>
+      <c r="G11" s="90">
+        <v>0.57843100000000003</v>
+      </c>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90">
+        <v>0.58354600000000001</v>
+      </c>
+      <c r="J11">
+        <v>0.60826899999999995</v>
+      </c>
+      <c r="K11">
+        <v>0.55370799999999998</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11" s="90">
+        <v>0.57672599999999996</v>
+      </c>
+      <c r="N11">
+        <v>0.60826899999999995</v>
+      </c>
+      <c r="O11">
+        <v>0.55370799999999998</v>
+      </c>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11">
+        <v>0.629</v>
+      </c>
+      <c r="S11">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="T11" s="88"/>
+      <c r="U11" s="88"/>
+    </row>
+    <row r="12" spans="2:21">
+      <c r="C12" s="90">
+        <v>0.56733299999999998</v>
+      </c>
+      <c r="D12" s="90">
+        <v>0.58543900000000004</v>
+      </c>
+      <c r="E12" s="90">
+        <v>0.61712599999999995</v>
+      </c>
+      <c r="F12" s="90">
+        <v>0.59637899999999999</v>
+      </c>
+      <c r="G12" s="90">
+        <v>0.56393800000000005</v>
+      </c>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90">
+        <v>0.59487000000000001</v>
+      </c>
+      <c r="J12">
+        <v>0.589036</v>
+      </c>
+      <c r="K12">
+        <v>0.558979</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12" s="90">
+        <v>0.58996599999999999</v>
+      </c>
+      <c r="N12">
+        <v>0.589036</v>
+      </c>
+      <c r="O12">
+        <v>0.558979</v>
+      </c>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="S12" s="68">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="T12" s="88"/>
+      <c r="U12" s="88"/>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="C13" s="90">
+        <v>0.67964999999999998</v>
+      </c>
+      <c r="D13" s="90">
+        <v>0.68577699999999997</v>
+      </c>
+      <c r="E13" s="90">
+        <v>0.65908100000000003</v>
+      </c>
+      <c r="F13" s="90">
+        <v>0.68402600000000002</v>
+      </c>
+      <c r="G13" s="90">
+        <v>0.68884000000000001</v>
+      </c>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90">
+        <v>0.64682700000000004</v>
+      </c>
+      <c r="J13">
+        <v>0.72643599999999997</v>
+      </c>
+      <c r="K13">
+        <v>0.63371299999999997</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13" s="90">
+        <v>0.63457300000000005</v>
+      </c>
+      <c r="N13">
+        <v>0.72643599999999997</v>
+      </c>
+      <c r="O13">
+        <v>0.63371299999999997</v>
+      </c>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13" s="68">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="T13" s="88"/>
+      <c r="U13" s="88"/>
+    </row>
+    <row r="14" spans="2:21">
+      <c r="C14" s="90">
+        <v>0.62041800000000003</v>
+      </c>
+      <c r="D14" s="90">
+        <v>0.60780400000000001</v>
+      </c>
+      <c r="E14" s="90">
+        <v>0.62041800000000003</v>
+      </c>
+      <c r="F14" s="90">
+        <v>0.60583399999999998</v>
+      </c>
+      <c r="G14" s="90">
+        <v>0.62790699999999999</v>
+      </c>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90">
+        <v>0.60780400000000001</v>
+      </c>
+      <c r="J14">
+        <v>0.62865000000000004</v>
+      </c>
+      <c r="K14">
+        <v>0.58089999999999997</v>
+      </c>
+      <c r="L14"/>
+      <c r="M14" s="90">
+        <v>0.60543899999999995</v>
+      </c>
+      <c r="N14">
+        <v>0.62865000000000004</v>
+      </c>
+      <c r="O14">
+        <v>0.58168900000000001</v>
+      </c>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="S14">
+        <v>0.62</v>
+      </c>
+      <c r="T14" s="88"/>
+      <c r="U14" s="88"/>
+    </row>
+    <row r="15" spans="2:21">
+      <c r="C15" s="90">
+        <v>0.57034200000000002</v>
+      </c>
+      <c r="D15" s="90">
+        <v>0.59526800000000002</v>
+      </c>
+      <c r="E15" s="90">
+        <v>0.46261099999999999</v>
+      </c>
+      <c r="F15" s="90">
+        <v>0.58639600000000003</v>
+      </c>
+      <c r="G15" s="90">
+        <v>0.53612199999999999</v>
+      </c>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90">
+        <v>0.59822600000000004</v>
+      </c>
+      <c r="J15">
+        <v>0.64807800000000004</v>
+      </c>
+      <c r="K15">
+        <v>0.59019900000000003</v>
+      </c>
+      <c r="L15"/>
+      <c r="M15" s="90">
+        <v>0.59231100000000003</v>
+      </c>
+      <c r="N15">
+        <v>0.64807800000000004</v>
+      </c>
+      <c r="O15">
+        <v>0.59019900000000003</v>
+      </c>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15" s="88"/>
+      <c r="U15" s="88"/>
+    </row>
+    <row r="16" spans="2:21">
+      <c r="C16" s="90">
+        <v>0.65446199999999999</v>
+      </c>
+      <c r="D16" s="90">
+        <v>0.64568999999999999</v>
+      </c>
+      <c r="E16" s="90">
+        <v>0.63958800000000005</v>
+      </c>
+      <c r="F16" s="90">
+        <v>0.62242600000000003</v>
+      </c>
+      <c r="G16" s="90">
+        <v>0.59839799999999999</v>
+      </c>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90">
+        <v>0.62318799999999996</v>
+      </c>
+      <c r="J16">
+        <v>0.68195700000000004</v>
+      </c>
+      <c r="K16">
+        <v>0.62366200000000005</v>
+      </c>
+      <c r="L16"/>
+      <c r="M16" s="90">
+        <v>0.61861200000000005</v>
+      </c>
+      <c r="N16">
+        <v>0.68195700000000004</v>
+      </c>
+      <c r="O16">
+        <v>0.62366200000000005</v>
+      </c>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16" s="88"/>
+      <c r="U16" s="88"/>
+    </row>
+    <row r="17" spans="2:21">
+      <c r="C17" s="90">
+        <v>0.41425099999999998</v>
+      </c>
+      <c r="D17" s="90">
+        <v>0.64412199999999997</v>
+      </c>
+      <c r="E17" s="90">
+        <v>0.56401000000000001</v>
+      </c>
+      <c r="F17" s="90">
+        <v>0.65378400000000003</v>
+      </c>
+      <c r="G17" s="90">
+        <v>0.53059599999999996</v>
+      </c>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90">
+        <v>0.65418699999999996</v>
+      </c>
+      <c r="J17">
+        <v>0.66209700000000005</v>
+      </c>
+      <c r="K17">
+        <v>0.62419400000000003</v>
+      </c>
+      <c r="L17"/>
+      <c r="M17" s="90">
+        <v>0.64975799999999995</v>
+      </c>
+      <c r="N17">
+        <v>0.66209700000000005</v>
+      </c>
+      <c r="O17">
+        <v>0.62419400000000003</v>
+      </c>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17" s="88"/>
+      <c r="U17" s="88"/>
+    </row>
+    <row r="18" spans="2:21">
+      <c r="C18" s="90">
+        <v>0.53059500000000004</v>
+      </c>
+      <c r="D18" s="90">
+        <v>0.62088100000000002</v>
+      </c>
+      <c r="E18" s="90">
+        <v>0.62387700000000001</v>
+      </c>
+      <c r="F18" s="90">
+        <v>0.621309</v>
+      </c>
+      <c r="G18" s="90">
+        <v>0.59606300000000001</v>
+      </c>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90">
+        <v>0.62173699999999998</v>
+      </c>
+      <c r="J18">
+        <v>0.63029500000000005</v>
+      </c>
+      <c r="K18">
+        <v>0.54514300000000004</v>
+      </c>
+      <c r="L18"/>
+      <c r="M18" s="90">
+        <v>0.60290999999999995</v>
+      </c>
+      <c r="N18">
+        <v>0.63029500000000005</v>
+      </c>
+      <c r="O18">
+        <v>0.54899399999999998</v>
+      </c>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18" s="88"/>
+      <c r="U18" s="88"/>
+    </row>
+    <row r="19" spans="2:21">
+      <c r="B19" s="68" t="s">
+        <v>263</v>
+      </c>
+      <c r="C19" s="88">
+        <f>AVERAGE(C4:C18)</f>
+        <v>0.58511719999999989</v>
+      </c>
+      <c r="D19" s="88">
+        <f t="shared" ref="D19:K19" si="0">AVERAGE(D4:D18)</f>
+        <v>0.61911633333333327</v>
+      </c>
+      <c r="E19" s="88">
+        <f t="shared" si="0"/>
+        <v>0.60451900000000003</v>
+      </c>
+      <c r="F19" s="88">
+        <f t="shared" si="0"/>
+        <v>0.61773553333333331</v>
+      </c>
+      <c r="G19" s="88">
+        <f t="shared" si="0"/>
+        <v>0.5953495333333334</v>
+      </c>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88">
+        <f t="shared" si="0"/>
+        <v>0.61533566666666661</v>
+      </c>
+      <c r="J19" s="88">
+        <f t="shared" si="0"/>
+        <v>0.65044573333333333</v>
+      </c>
+      <c r="K19" s="88">
+        <f t="shared" si="0"/>
+        <v>0.5899728666666666</v>
+      </c>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88">
+        <f t="shared" ref="M19" si="1">AVERAGE(M4:M18)</f>
+        <v>0.61240573333333315</v>
+      </c>
+      <c r="N19" s="88">
+        <f t="shared" ref="N19" si="2">AVERAGE(N4:N18)</f>
+        <v>0.65044573333333333</v>
+      </c>
+      <c r="O19" s="88">
+        <f t="shared" ref="O19" si="3">AVERAGE(O4:O18)</f>
+        <v>0.5903084666666667</v>
+      </c>
+      <c r="P19" s="88"/>
+      <c r="Q19" s="88"/>
+      <c r="R19" s="88"/>
+      <c r="S19" s="88"/>
+      <c r="T19" s="88"/>
+      <c r="U19" s="88"/>
+    </row>
+    <row r="20" spans="2:21">
+      <c r="B20" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" s="88">
+        <f>_xlfn.STDEV.P(C4:C18)</f>
+        <v>8.0893369974059881E-2</v>
+      </c>
+      <c r="D20" s="88">
+        <f t="shared" ref="D20:K20" si="4">_xlfn.STDEV.P(D4:D18)</f>
+        <v>4.2484831705235947E-2</v>
+      </c>
+      <c r="E20" s="88">
+        <f t="shared" si="4"/>
+        <v>5.4256432225743223E-2</v>
+      </c>
+      <c r="F20" s="88">
+        <f t="shared" si="4"/>
+        <v>4.1497096878161922E-2</v>
+      </c>
+      <c r="G20" s="88">
+        <f t="shared" si="4"/>
+        <v>5.5783090577541702E-2</v>
+      </c>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88">
+        <f t="shared" si="4"/>
+        <v>3.273574932631839E-2</v>
+      </c>
+      <c r="J20" s="88">
+        <f t="shared" si="4"/>
+        <v>4.2476846722995912E-2</v>
+      </c>
+      <c r="K20" s="88">
+        <f t="shared" si="4"/>
+        <v>3.238028985224739E-2</v>
+      </c>
+      <c r="L20" s="88"/>
+      <c r="M20" s="88">
+        <f>_xlfn.STDEV.P(M4:M18)</f>
+        <v>3.0178871110909528E-2</v>
+      </c>
+      <c r="N20" s="88">
+        <f>_xlfn.STDEV.P(N4:N18)</f>
+        <v>4.2476846722995912E-2</v>
+      </c>
+      <c r="O20" s="88">
+        <f>_xlfn.STDEV.P(O4:O18)</f>
+        <v>3.1999533425487454E-2</v>
+      </c>
+      <c r="P20" s="88"/>
+      <c r="Q20" s="88"/>
+      <c r="R20" s="88"/>
+      <c r="S20" s="88"/>
+      <c r="T20" s="88"/>
+      <c r="U20" s="88"/>
+    </row>
+    <row r="21" spans="2:21">
+      <c r="B21" s="68" t="s">
+        <v>268</v>
+      </c>
+      <c r="C21" s="68">
+        <f>MEDIAN(C4:C18)</f>
+        <v>0.59196499999999996</v>
+      </c>
+      <c r="D21" s="68">
+        <f t="shared" ref="D21:O21" si="5">MEDIAN(D4:D18)</f>
+        <v>0.60780400000000001</v>
+      </c>
+      <c r="E21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.60803099999999999</v>
+      </c>
+      <c r="F21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.60583399999999998</v>
+      </c>
+      <c r="G21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.57843100000000003</v>
+      </c>
+      <c r="I21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.60780400000000001</v>
+      </c>
+      <c r="J21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.64078400000000002</v>
+      </c>
+      <c r="K21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.59019900000000003</v>
+      </c>
+      <c r="M21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.60543899999999995</v>
+      </c>
+      <c r="N21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.64078400000000002</v>
+      </c>
+      <c r="O21" s="68">
+        <f t="shared" si="5"/>
+        <v>0.59019900000000003</v>
+      </c>
+      <c r="Q21" s="68">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="S21" s="68">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="T21" s="88"/>
+      <c r="U21" s="88"/>
+    </row>
+    <row r="22" spans="2:21">
+      <c r="B22" s="89" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="90">
+        <v>0.59173600000000004</v>
+      </c>
+      <c r="D22" s="90">
+        <v>0.55495899999999998</v>
+      </c>
+      <c r="E22" s="90">
+        <v>0.556612</v>
+      </c>
+      <c r="F22" s="90">
+        <v>0.59421500000000005</v>
+      </c>
+      <c r="G22" s="90">
+        <v>0.60743800000000003</v>
+      </c>
+      <c r="H22" s="90"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22" s="88"/>
+      <c r="U22" s="88"/>
+    </row>
+    <row r="23" spans="2:21">
+      <c r="C23" s="90">
+        <v>0.56844099999999997</v>
+      </c>
+      <c r="D23" s="90">
+        <v>0.60722399999999999</v>
+      </c>
+      <c r="E23" s="90">
+        <v>0.477186</v>
+      </c>
+      <c r="F23" s="90">
+        <v>0.56920199999999999</v>
+      </c>
+      <c r="G23" s="90">
+        <v>0.56958200000000003</v>
+      </c>
+      <c r="H23" s="90"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23" s="88"/>
+      <c r="U23" s="88"/>
+    </row>
+    <row r="24" spans="2:21">
+      <c r="C24" s="90">
+        <v>0.58369400000000005</v>
+      </c>
+      <c r="D24" s="90">
+        <v>0.56124499999999999</v>
+      </c>
+      <c r="E24" s="90">
+        <v>0.59826699999999999</v>
+      </c>
+      <c r="F24" s="90">
+        <v>0.58487599999999995</v>
+      </c>
+      <c r="G24" s="90">
+        <v>0.58448199999999995</v>
+      </c>
+      <c r="H24" s="90"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24" s="88"/>
+      <c r="U24" s="88"/>
+    </row>
+    <row r="25" spans="2:21">
+      <c r="C25" s="90">
+        <v>0.745726</v>
+      </c>
+      <c r="D25" s="90">
+        <v>0.73717900000000003</v>
+      </c>
+      <c r="E25" s="90">
+        <v>0.70555599999999996</v>
+      </c>
+      <c r="F25" s="90">
+        <v>0.71495699999999995</v>
+      </c>
+      <c r="G25" s="90">
+        <v>0.70769199999999999</v>
+      </c>
+      <c r="H25" s="90"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25" s="88"/>
+      <c r="U25" s="88"/>
+    </row>
+    <row r="26" spans="2:21">
+      <c r="C26" s="90">
+        <v>0.64144100000000004</v>
+      </c>
+      <c r="D26" s="90">
+        <v>0.63496600000000003</v>
+      </c>
+      <c r="E26" s="90">
+        <v>0.63698900000000003</v>
+      </c>
+      <c r="F26" s="90">
+        <v>0.63941700000000001</v>
+      </c>
+      <c r="G26" s="90">
+        <v>0.60946999999999996</v>
+      </c>
+      <c r="H26" s="90"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26" s="88"/>
+      <c r="U26" s="88"/>
+    </row>
+    <row r="27" spans="2:21">
+      <c r="C27" s="90">
+        <v>0.56992799999999999</v>
+      </c>
+      <c r="D27" s="90">
+        <v>0.58514500000000003</v>
+      </c>
+      <c r="E27" s="90">
+        <v>0.578623</v>
+      </c>
+      <c r="F27" s="90">
+        <v>0.58297100000000002</v>
+      </c>
+      <c r="G27" s="90">
+        <v>0.57644899999999999</v>
+      </c>
+      <c r="H27" s="90"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27" s="88"/>
+      <c r="U27" s="88"/>
+    </row>
+    <row r="28" spans="2:21">
+      <c r="C28" s="90">
+        <v>0.62287199999999998</v>
+      </c>
+      <c r="D28" s="90">
+        <v>0.62374499999999999</v>
+      </c>
+      <c r="E28" s="90">
+        <v>0.61719800000000002</v>
+      </c>
+      <c r="F28" s="90">
+        <v>0.61894400000000005</v>
+      </c>
+      <c r="G28" s="90">
+        <v>0.60672199999999998</v>
+      </c>
+      <c r="H28" s="90"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28" s="88"/>
+      <c r="U28" s="88"/>
+    </row>
+    <row r="29" spans="2:21">
+      <c r="C29" s="90">
+        <v>0.61082700000000001</v>
+      </c>
+      <c r="D29" s="90">
+        <v>0.60017100000000001</v>
+      </c>
+      <c r="E29" s="90">
+        <v>0.59249799999999997</v>
+      </c>
+      <c r="F29" s="90">
+        <v>0.59036699999999998</v>
+      </c>
+      <c r="G29" s="90">
+        <v>0.57885799999999998</v>
+      </c>
+      <c r="H29" s="90"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29" s="88"/>
+      <c r="U29" s="88"/>
+    </row>
+    <row r="30" spans="2:21">
+      <c r="C30" s="90">
+        <v>0.57299100000000003</v>
+      </c>
+      <c r="D30" s="90">
+        <v>0.58128999999999997</v>
+      </c>
+      <c r="E30" s="90">
+        <v>0.57978099999999999</v>
+      </c>
+      <c r="F30" s="90">
+        <v>0.59411499999999995</v>
+      </c>
+      <c r="G30" s="90">
+        <v>0.62617900000000004</v>
+      </c>
+      <c r="H30" s="90"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30" s="88"/>
+      <c r="U30" s="88"/>
+    </row>
+    <row r="31" spans="2:21">
+      <c r="C31" s="90">
+        <v>0.66827099999999995</v>
+      </c>
+      <c r="D31" s="90">
+        <v>0.68140000000000001</v>
+      </c>
+      <c r="E31" s="90">
+        <v>0.65995599999999999</v>
+      </c>
+      <c r="F31" s="90">
+        <v>0.67527400000000004</v>
+      </c>
+      <c r="G31" s="90">
+        <v>0.66608299999999998</v>
+      </c>
+      <c r="H31" s="90"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31" s="88"/>
+      <c r="U31" s="88"/>
+    </row>
+    <row r="32" spans="2:21">
+      <c r="C32" s="90">
+        <v>0.61765899999999996</v>
+      </c>
+      <c r="D32" s="90">
+        <v>0.610958</v>
+      </c>
+      <c r="E32" s="90">
+        <v>0.60859300000000005</v>
+      </c>
+      <c r="F32" s="90">
+        <v>0.61805299999999996</v>
+      </c>
+      <c r="G32" s="90">
+        <v>0.63184899999999999</v>
+      </c>
+      <c r="H32" s="90"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32" s="88"/>
+      <c r="U32" s="88"/>
+    </row>
+    <row r="33" spans="2:21">
+      <c r="C33" s="90">
+        <v>0.58681899999999998</v>
+      </c>
+      <c r="D33" s="90">
+        <v>0.59780299999999997</v>
+      </c>
+      <c r="E33" s="90">
+        <v>0.57498899999999997</v>
+      </c>
+      <c r="F33" s="90">
+        <v>0.58090399999999998</v>
+      </c>
+      <c r="G33" s="90">
+        <v>0.55935800000000002</v>
+      </c>
+      <c r="H33" s="90"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33" s="88"/>
+      <c r="U33" s="88"/>
+    </row>
+    <row r="34" spans="2:21">
+      <c r="C34" s="90">
+        <v>0.64759699999999998</v>
+      </c>
+      <c r="D34" s="90">
+        <v>0.652555</v>
+      </c>
+      <c r="E34" s="90">
+        <v>0.63348599999999999</v>
+      </c>
+      <c r="F34" s="90">
+        <v>0.62395100000000003</v>
+      </c>
+      <c r="G34" s="90">
+        <v>0.59763500000000003</v>
+      </c>
+      <c r="H34" s="90"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34" s="88"/>
+      <c r="U34" s="88"/>
+    </row>
+    <row r="35" spans="2:21">
+      <c r="C35" s="90">
+        <v>0.53542699999999999</v>
+      </c>
+      <c r="D35" s="90">
+        <v>0.63607100000000005</v>
+      </c>
+      <c r="E35" s="90">
+        <v>0.53542699999999999</v>
+      </c>
+      <c r="F35" s="90">
+        <v>0.60346200000000005</v>
+      </c>
+      <c r="G35" s="90">
+        <v>0.62560400000000005</v>
+      </c>
+      <c r="H35" s="90"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35" s="88"/>
+      <c r="U35" s="88"/>
+    </row>
+    <row r="36" spans="2:21">
+      <c r="C36" s="90">
+        <v>0.61745799999999995</v>
+      </c>
+      <c r="D36" s="90">
+        <v>0.61446299999999998</v>
+      </c>
+      <c r="E36" s="90">
+        <v>0.60633300000000001</v>
+      </c>
+      <c r="F36" s="90">
+        <v>0.61745799999999995</v>
+      </c>
+      <c r="G36" s="90">
+        <v>0.61702999999999997</v>
+      </c>
+      <c r="H36" s="90"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36" s="88"/>
+      <c r="U36" s="88"/>
+    </row>
+    <row r="37" spans="2:21">
+      <c r="B37" s="68" t="s">
+        <v>263</v>
+      </c>
+      <c r="C37" s="88">
+        <f>AVERAGE(C22:C36)</f>
+        <v>0.61205913333333328</v>
+      </c>
+      <c r="D37" s="88">
+        <f t="shared" ref="D37" si="6">AVERAGE(D22:D36)</f>
+        <v>0.61861159999999993</v>
+      </c>
+      <c r="E37" s="88">
+        <f t="shared" ref="E37" si="7">AVERAGE(E22:E36)</f>
+        <v>0.59743293333333325</v>
+      </c>
+      <c r="F37" s="88">
+        <f t="shared" ref="F37" si="8">AVERAGE(F22:F36)</f>
+        <v>0.61387773333333329</v>
+      </c>
+      <c r="G37" s="88">
+        <f t="shared" ref="G37" si="9">AVERAGE(G22:G36)</f>
+        <v>0.61096206666666675</v>
+      </c>
+      <c r="H37" s="88"/>
+      <c r="M37" s="88"/>
+      <c r="N37" s="88"/>
+      <c r="O37" s="88"/>
+      <c r="P37" s="88"/>
+      <c r="Q37" s="88"/>
+      <c r="R37" s="88"/>
+      <c r="S37" s="88"/>
+    </row>
+    <row r="38" spans="2:21">
+      <c r="B38" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" s="88">
+        <f>_xlfn.STDEV.P(C22:C36)</f>
+        <v>4.9168305158054357E-2</v>
+      </c>
+      <c r="D38" s="88">
+        <f t="shared" ref="D38:G38" si="10">_xlfn.STDEV.P(D22:D36)</f>
+        <v>4.5155604790250943E-2</v>
+      </c>
+      <c r="E38" s="88">
+        <f t="shared" si="10"/>
+        <v>5.1783682523186991E-2</v>
+      </c>
+      <c r="F38" s="88">
+        <f t="shared" si="10"/>
+        <v>3.751809208629292E-2</v>
+      </c>
+      <c r="G38" s="88">
+        <f t="shared" si="10"/>
+        <v>3.7258165062111624E-2</v>
+      </c>
+      <c r="H38" s="88"/>
+      <c r="M38" s="88"/>
+      <c r="N38" s="88"/>
+      <c r="O38" s="88"/>
+      <c r="P38" s="88"/>
+      <c r="Q38" s="88"/>
+      <c r="R38" s="88"/>
+      <c r="S38" s="88"/>
+    </row>
+    <row r="39" spans="2:21">
+      <c r="F39" s="88"/>
+      <c r="G39" s="88"/>
+      <c r="H39" s="88"/>
+      <c r="I39" s="88"/>
+      <c r="J39" s="88"/>
+      <c r="K39" s="88"/>
+      <c r="L39" s="88"/>
+      <c r="M39" s="88"/>
+      <c r="N39" s="88"/>
+      <c r="O39" s="88"/>
+      <c r="P39" s="88"/>
+      <c r="Q39" s="88"/>
+      <c r="R39" s="88"/>
+      <c r="S39" s="88"/>
+    </row>
+    <row r="40" spans="2:21">
+      <c r="F40" s="88"/>
+      <c r="G40" s="88"/>
+      <c r="H40" s="88"/>
+      <c r="I40" s="88"/>
+      <c r="J40" s="88"/>
+      <c r="K40" s="88"/>
+      <c r="L40" s="88"/>
+      <c r="M40" s="88"/>
+      <c r="N40" s="88"/>
+      <c r="O40" s="88"/>
+      <c r="P40" s="88"/>
+      <c r="Q40" s="88"/>
+      <c r="R40" s="88"/>
+      <c r="S40" s="88"/>
+    </row>
+    <row r="41" spans="2:21">
+      <c r="F41" s="88"/>
+      <c r="G41" s="88"/>
+      <c r="H41" s="88"/>
+      <c r="I41" s="88"/>
+      <c r="J41" s="88"/>
+      <c r="K41" s="88"/>
+      <c r="L41" s="88"/>
+      <c r="M41" s="88"/>
+      <c r="N41" s="88"/>
+      <c r="O41" s="88"/>
+      <c r="P41" s="88"/>
+      <c r="Q41" s="88"/>
+      <c r="R41" s="88"/>
+      <c r="S41" s="88"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9614E59-38A6-4E72-A048-1249DD807382}">
   <dimension ref="B1:H14"/>
@@ -14285,29 +16893,29 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="8"/>
-    <col min="2" max="2" width="15.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="8"/>
+    <col min="2" max="2" width="15.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" style="8" customWidth="1"/>
     <col min="4" max="4" width="35" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="20.453125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.5546875" style="8"/>
+    <col min="14" max="16384" width="11.54296875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1"/>
     <row r="2" spans="2:8" ht="15" thickBot="1">
-      <c r="B2" s="88"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
       <c r="E2" s="87" t="s">
         <v>247</v>
       </c>
@@ -14561,30 +17169,30 @@
       <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.77734375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7265625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.54296875" hidden="1" customWidth="1"/>
     <col min="17" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="55.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="55.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.54296875" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="17.7265625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="38" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="41.26953125" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.109375" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16837,31 +19445,31 @@
       <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.77734375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7265625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15.54296875" hidden="1" customWidth="1"/>
     <col min="17" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="55.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="55.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.54296875" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="17.7265625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="41.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.1796875" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="0" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.109375" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19107,43 +21715,43 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" customWidth="1"/>
-    <col min="13" max="13" width="8.21875" customWidth="1"/>
-    <col min="14" max="14" width="8.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="93" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90" t="s">
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
     </row>
-    <row r="2" spans="1:14" ht="57.6">
+    <row r="2" spans="1:14" ht="43.5">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -20785,11 +23393,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A97" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q94" sqref="Q94"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD119" sqref="AD119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
@@ -20805,20 +23413,20 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="1" max="1" width="1.7265625" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" customWidth="1"/>
+    <col min="3" max="3" width="55.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1"/>
-    <row r="2" spans="2:8" ht="29.4" thickBot="1">
+    <row r="2" spans="2:8" ht="29.5" thickBot="1">
       <c r="B2" s="20"/>
       <c r="C2" s="17" t="s">
         <v>177</v>
@@ -20839,7 +23447,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="28.8">
+    <row r="3" spans="2:8" ht="29">
       <c r="B3" s="21" t="s">
         <v>183</v>
       </c>
@@ -20868,7 +23476,7 @@
         <v>7.7070999145507804</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="29.4" thickBot="1">
+    <row r="4" spans="2:8" ht="29.5" thickBot="1">
       <c r="B4" s="22" t="s">
         <v>184</v>
       </c>
@@ -20907,14 +23515,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34546FC6-D57A-4B77-AEB4-856253278101}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -21079,7 +23687,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="94" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -21087,13 +23695,13 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="91"/>
+      <c r="A21" s="94"/>
       <c r="B21" s="4" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="91" t="s">
+      <c r="A22" s="94" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -21101,7 +23709,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="91"/>
+      <c r="A23" s="94"/>
       <c r="B23" s="4" t="s">
         <v>158</v>
       </c>
@@ -21147,7 +23755,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="91" t="s">
+      <c r="A29" s="94" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -21155,13 +23763,13 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="91"/>
+      <c r="A30" s="94"/>
       <c r="B30" s="4" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="91" t="s">
+      <c r="A31" s="94" t="s">
         <v>26</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -21169,7 +23777,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="91"/>
+      <c r="A32" s="94"/>
       <c r="B32" s="4" t="s">
         <v>166</v>
       </c>
@@ -21205,16 +23813,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7230CB46-5D11-49E2-8F2E-F48D49BF63C3}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="18.33203125" customWidth="1"/>
+    <col min="4" max="6" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -21275,7 +23883,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="95" t="s">
         <v>253</v>
       </c>
       <c r="B5" s="71" t="s">
@@ -21290,7 +23898,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="92"/>
+      <c r="A6" s="95"/>
       <c r="B6" s="71" t="s">
         <v>245</v>
       </c>
@@ -21303,7 +23911,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="92"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="71" t="s">
         <v>246</v>
       </c>
@@ -21316,7 +23924,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="92"/>
+      <c r="A8" s="95"/>
       <c r="B8" s="71" t="s">
         <v>236</v>
       </c>
@@ -21385,7 +23993,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="15" thickBot="1"/>
-    <row r="18" spans="2:6" ht="43.2">
+    <row r="18" spans="2:6" ht="43.5">
       <c r="B18" s="62"/>
       <c r="C18" s="82" t="s">
         <v>240</v>

</xml_diff>